<commit_message>
modal types function added
</commit_message>
<xml_diff>
--- a/data/type-descriptions/siblings.xlsx
+++ b/data/type-descriptions/siblings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sp16194/Google Drive/UniWork/projects/kinspace-systems/code/results/type-descriptions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u1123114/Documents/projects/kinspace/data/type-descriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD80ECA-66B0-874B-AC2B-4A38D11F4224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11111BC9-32CF-A543-9A5C-A4C073AD4AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{23A97693-A90F-BA42-A45B-354D964D23DA}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{23A97693-A90F-BA42-A45B-354D964D23DA}"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="1" r:id="rId1"/>
@@ -199,7 +199,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -554,14 +554,14 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="71.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +578,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -595,7 +595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -612,7 +612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -629,7 +629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -646,7 +646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -663,7 +663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -680,7 +680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -697,7 +697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -714,7 +714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -731,7 +731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -748,7 +748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -765,7 +765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -782,7 +782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -799,7 +799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -816,7 +816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -833,7 +833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
@@ -863,9 +863,12 @@
       <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="114.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="409.6">
+    <row r="1" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>

</xml_diff>